<commit_message>
added 3 more company data
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\Text Files\ajay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\codencode-site\Code-N-Code.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F57E8E-79C0-4CEF-BF20-E66498150C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3508DC14-5987-4229-8C3F-FF7C4F8F6A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t>Company Name</t>
   </si>
@@ -164,13 +164,99 @@
   </si>
   <si>
     <t>Website</t>
+  </si>
+  <si>
+    <t>Lenskart Solutions Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Lenskart</t>
+  </si>
+  <si>
+    <t>U33100DL2008PTC178355</t>
+  </si>
+  <si>
+    <t>Internet Retail, Speciality Retail</t>
+  </si>
+  <si>
+    <t>Lenskart, founded in 2008, is an Indian eyewear company operating through both online and offline channels. The business designs, manufactures, and retails prescription glasses, sunglasses, and contact lenses. By integrating technology with retail operations, it provides services such as virtual try-ons and home eye tests, positioning itself as a significant player in the organized eyewear market.</t>
+  </si>
+  <si>
+    <t>W-123, Greater Kailash Part-2 , New Delhi, Delhi, India - 110048.</t>
+  </si>
+  <si>
+    <t>support@lenskart.com</t>
+  </si>
+  <si>
+    <t>https://www.lenskart.com/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/lenskart-com/?originalSubdomain=in</t>
+  </si>
+  <si>
+    <t>Honasa Consumer Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mamaearth, The Derma Co, Bblunt, Dr Sheth’s, Aqualogica, Staze 9to9, Bblunt Salons
+</t>
+  </si>
+  <si>
+    <t>L74999DL2016PLC306016</t>
+  </si>
+  <si>
+    <t>Personal Care Products, Internet Retail</t>
+  </si>
+  <si>
+    <t>Founded in September 2016, Mamaearth is a digital-first Indian beauty and personal care brand operating under Honasa Consumer Ltd. It offers toxin-free and Made Safe–certified products across categories like baby care, skincare, haircare, and cosmetics. Leveraging influencer marketing and omnichannel retail—including e-commerce marketplaces and physical outlets—it targets millennials seeking natural and safe personal care solutions</t>
+  </si>
+  <si>
+    <t>Unit No - 404, 4th Floor, City Centre, Plot No 05, Sector-12, Dwarka, South West Delhi, New Delhi, Delhi, India, 110075</t>
+  </si>
+  <si>
+    <t>https://honasa.in/
+https://mamaearth.in/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/honasa-consumer-ltd/</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/xml-data/corpfiling/AttachHis/f7192a9f-5721-412b-b388-9c6e93caa50e.pdf</t>
+  </si>
+  <si>
+    <t>Eternal Ltd.</t>
+  </si>
+  <si>
+    <t>Zomato, Blinkit, District, Feeding India, Hyperpure, Zomato Live, Zomaland, Weather Union</t>
+  </si>
+  <si>
+    <t>L93030DL2010PLC198141</t>
+  </si>
+  <si>
+    <t>Interactive Media &amp; Services, FoodTech</t>
+  </si>
+  <si>
+    <t>Eternal Ltd., established in 2010 as Zomato, is an Indian public company headquartered in Gurugram. It operates a diversified platform comprising food delivery (Zomato), quick-commerce (Blinkit), B2B food supplies (Hyperpure), and event ticketing (Zomato Live/District). The company connects consumers and businesses through digital services, combining logistics, procurement, and entertainment under a technology-driven model.</t>
+  </si>
+  <si>
+    <t>Ground Floor 12a, 94 Meghdoot Nehru Place, South Delhi, New Delhi, Delhi, India, 110019</t>
+  </si>
+  <si>
+    <t>Pioneer Square, Sector 62, Golf Course Extension Road, Gurugram, Haryana 122101</t>
+  </si>
+  <si>
+    <t>info@zomato.com</t>
+  </si>
+  <si>
+    <t>https://www.zomato.com/</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/xml-data/corpfiling/AttachHis/e2687a83-7148-436f-9c29-f2d06f912134.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,16 +286,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF474747"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="MyFirstFont"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,12 +350,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -250,6 +383,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -555,13 +718,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
@@ -585,7 +748,7 @@
     <col min="21" max="21" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -709,7 +872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" thickBot="1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -769,6 +932,167 @@
       </c>
       <c r="U3" s="5" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="29.4" thickBot="1">
+      <c r="A4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="7">
+        <v>39811</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="9">
+        <v>8929173142</v>
+      </c>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="1:21" ht="72.599999999999994" thickBot="1">
+      <c r="A5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="7">
+        <v>42629</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="14">
+        <v>544014</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="9">
+        <v>8901555444</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="58.2" thickBot="1">
+      <c r="A6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="7">
+        <v>40196</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="15">
+        <v>543320</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="T6" s="6"/>
+      <c r="U6" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -779,8 +1103,14 @@
     <hyperlink ref="T2" r:id="rId4" xr:uid="{3A8FC6ED-6B3A-47CE-8BDB-0E2FCACF3338}"/>
     <hyperlink ref="T3" r:id="rId5" xr:uid="{F311E69E-80FA-4FD0-B58F-A05A2F6A8159}"/>
     <hyperlink ref="U3" r:id="rId6" xr:uid="{202D526D-454F-4306-BCFF-D58CA9B766A1}"/>
+    <hyperlink ref="S4" r:id="rId7" xr:uid="{905701BC-F975-4D0A-B23F-FB4F2F36DC0D}"/>
+    <hyperlink ref="T4" r:id="rId8" xr:uid="{F71AAF24-C891-4FCA-9CAC-43CC714FBCB5}"/>
+    <hyperlink ref="T5" r:id="rId9" xr:uid="{BFEA703C-576F-4ADE-B7B7-DA45A5D3BEFE}"/>
+    <hyperlink ref="U5" r:id="rId10" xr:uid="{CF2FB9B2-4AD0-4339-B08D-D48E55484907}"/>
+    <hyperlink ref="S6" r:id="rId11" xr:uid="{8712A85A-E5C7-4922-95B3-95CE20CF7C84}"/>
+    <hyperlink ref="U6" r:id="rId12" xr:uid="{FF2FF4A2-FFD8-46D9-907D-65CAC3E55A0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected date format ini xls file.
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\codencode-site\Code-N-Code.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3508DC14-5987-4229-8C3F-FF7C4F8F6A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E666648-C7A1-4E56-BD81-F8179450911A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t>Company Name</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>https://www.bseindia.com/xml-data/corpfiling/AttachHis/e2687a83-7148-436f-9c29-f2d06f912134.pdf</t>
+  </si>
+  <si>
+    <t>29 Dec 2008</t>
+  </si>
+  <si>
+    <t>16 Sep 2016</t>
+  </si>
+  <si>
+    <t>18 Jan 2010</t>
   </si>
 </sst>
 </file>
@@ -370,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -386,9 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -412,6 +418,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -721,7 +736,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -729,7 +744,7 @@
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" style="4" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -758,7 +773,7 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -820,7 +835,7 @@
       <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
@@ -882,7 +897,7 @@
       <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
@@ -944,8 +959,8 @@
       <c r="C4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="7">
-        <v>39811</v>
+      <c r="D4" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>15</v>
@@ -961,26 +976,26 @@
       <c r="J4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>52</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>53</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>8929173142</v>
       </c>
       <c r="Q4" s="6"/>
-      <c r="R4" s="10" t="s">
+      <c r="R4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="T4" s="12" t="s">
         <v>56</v>
       </c>
       <c r="U4" s="6"/>
@@ -995,8 +1010,8 @@
       <c r="C5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="7">
-        <v>42629</v>
+      <c r="D5" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -1007,7 +1022,7 @@
       <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>544014</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -1016,27 +1031,27 @@
       <c r="J5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>61</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>62</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>8901555444</v>
       </c>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-      <c r="S5" s="11" t="s">
+      <c r="S5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="12" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1050,8 +1065,8 @@
       <c r="C6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="7">
-        <v>40196</v>
+      <c r="D6" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -1062,7 +1077,7 @@
       <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>543320</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -1071,27 +1086,27 @@
       <c r="J6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>70</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>72</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="S6" s="12" t="s">
         <v>74</v>
       </c>
       <c r="T6" s="6"/>
-      <c r="U6" s="13" t="s">
+      <c r="U6" s="12" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>